<commit_message>
began writing report and changed table during lab session
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\Stage_5\Digital_and_Embedded_Systems_EEEN40280\Labs\Digital_and_Embedded_Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Stage_5\Digital_and_Embedded_Systems_EEEN40280\Labs\Digital_and_Embedded_Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Bit switches</t>
   </si>
@@ -56,16 +56,22 @@
     <t>High Byte Reload</t>
   </si>
   <si>
-    <t>Actual Reload Freq</t>
-  </si>
-  <si>
     <t>Speaker Freq</t>
+  </si>
+  <si>
+    <t>Low Byte Reload</t>
+  </si>
+  <si>
+    <t>Actual Interrupt Freq</t>
+  </si>
+  <si>
+    <t>Reload Values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,11 +383,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,12 +398,13 @@
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -417,13 +424,19 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -443,19 +456,26 @@
         <v>10240</v>
       </c>
       <c r="F2">
-        <f>ROUNDUP(E2/256,0)</f>
+        <f>ROUNDUP(E2/$A$11,0)</f>
         <v>40</v>
       </c>
       <c r="G2">
-        <f>ROUNDUP(11059200/(65536-(F2*256)),1)</f>
-        <v>200</v>
+        <v>128</v>
       </c>
       <c r="H2">
-        <f>ROUNDUP(G2/2,1)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f>F2*POWER(2,8)+G2</f>
+        <v>10368</v>
+      </c>
+      <c r="I2">
+        <f>ROUNDUP(11059200/(65536-H2),1)</f>
+        <v>200.5</v>
+      </c>
+      <c r="J2">
+        <f>ROUNDUP(I2/2,1)</f>
+        <v>100.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -475,19 +495,26 @@
         <v>43417</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F9" si="3">ROUNDUP(E3/256,0)</f>
+        <f t="shared" ref="F3:F9" si="3">ROUNDUP(E3/$A$11,0)</f>
         <v>170</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G9" si="4">ROUNDUP(11059200/(65536-(F3*256)),1)</f>
-        <v>502.40000000000003</v>
+        <v>128</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="5">ROUNDUP(G3/2,1)</f>
-        <v>251.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <f>F3*POWER(2,8)+G3</f>
+        <v>43648</v>
+      </c>
+      <c r="I3">
+        <f>ROUNDUP(11059200/(65536-H3),1)</f>
+        <v>505.3</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J9" si="4">ROUNDUP(I3/2,1)</f>
+        <v>252.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -511,15 +538,22 @@
         <v>213</v>
       </c>
       <c r="G4">
+        <v>128</v>
+      </c>
+      <c r="H4">
+        <f>F4*POWER(2,8)+G4</f>
+        <v>54656</v>
+      </c>
+      <c r="I4">
+        <f>ROUNDUP(11059200/(65536-H4),1)</f>
+        <v>1016.5</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="4"/>
-        <v>1004.7</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="5"/>
-        <v>502.40000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>508.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -543,140 +577,180 @@
         <v>235</v>
       </c>
       <c r="G5">
+        <v>128</v>
+      </c>
+      <c r="H5">
+        <f>F5*POWER(2,8)+G5</f>
+        <v>60288</v>
+      </c>
+      <c r="I5">
+        <f>ROUNDUP(11059200/(65536-H5),1)</f>
+        <v>2107.4</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="4"/>
-        <v>2057.1999999999998</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="5"/>
-        <v>1028.5999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1053.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>2765</v>
+        <v>3687</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>62771</v>
+        <v>61849</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G6">
+        <v>128</v>
+      </c>
+      <c r="H6">
+        <f>F6*POWER(2,8)+G6</f>
+        <v>62080</v>
+      </c>
+      <c r="I6">
+        <f>ROUNDUP(11059200/(65536-H6),1)</f>
+        <v>3200</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="4"/>
-        <v>4320</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="5"/>
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1844</v>
+        <v>2765</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>63692</v>
+        <v>62771</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G7">
+        <v>128</v>
+      </c>
+      <c r="H7">
+        <f>F7*POWER(2,8)+G7</f>
+        <v>63104</v>
+      </c>
+      <c r="I7">
+        <f>ROUNDUP(11059200/(65536-H7),1)</f>
+        <v>4547.4000000000005</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="4"/>
-        <v>6171.5</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="5"/>
-        <v>3085.7999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2273.6999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>1383</v>
+        <v>1844</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>64153</v>
+        <v>63692</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G8">
+        <v>128</v>
+      </c>
+      <c r="H8">
+        <f>F8*POWER(2,8)+G8</f>
+        <v>63872</v>
+      </c>
+      <c r="I8">
+        <f>ROUNDUP(11059200/(65536-H8),1)</f>
+        <v>6646.2000000000007</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="4"/>
-        <v>8640</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="5"/>
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3323.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>8000</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>1106</v>
+        <v>1383</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>64430</v>
+        <v>64153</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G9">
+        <v>128</v>
+      </c>
+      <c r="H9">
+        <f>F9*POWER(2,8)+G9</f>
+        <v>64384</v>
+      </c>
+      <c r="I9">
+        <f>ROUNDUP(11059200/(65536-H9),1)</f>
+        <v>9600</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="4"/>
-        <v>10800</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="5"/>
-        <v>5400</v>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -712,7 +786,7 @@
         <v>55536</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" ref="F20:F27" si="6">D20/256</f>
+        <f t="shared" ref="F20:F27" si="5">D20/256</f>
         <v>39.0625</v>
       </c>
       <c r="G20" s="1">
@@ -750,38 +824,38 @@
         <v>10000</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D27" si="7">C21+B21*A21</f>
+        <f t="shared" ref="D21:D27" si="6">C21+B21*A21</f>
         <v>17742</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E26" si="8">(65536)-D21</f>
+        <f t="shared" ref="E21:E26" si="7">(65536)-D21</f>
         <v>47794</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>69.3046875</v>
       </c>
       <c r="G21" s="1">
         <v>150</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H27" si="9">G21*256</f>
+        <f t="shared" ref="H21:H27" si="8">G21*256</f>
         <v>38400</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I27" si="10">65536-H21</f>
+        <f t="shared" ref="I21:I27" si="9">65536-H21</f>
         <v>27136</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:J27" si="11">(11059200)</f>
+        <f t="shared" ref="J21:J27" si="10">(11059200)</f>
         <v>11059200</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K27" si="12">I21/J21</f>
+        <f t="shared" ref="K21:K27" si="11">I21/J21</f>
         <v>2.4537037037037036E-3</v>
       </c>
       <c r="L21">
-        <f t="shared" ref="L21:L27" si="13">1/(2*K21)</f>
+        <f t="shared" ref="L21:L27" si="12">1/(2*K21)</f>
         <v>203.77358490566039</v>
       </c>
     </row>
@@ -796,38 +870,38 @@
         <v>10000</v>
       </c>
       <c r="D22">
+        <f t="shared" si="6"/>
+        <v>25484</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="7"/>
-        <v>25484</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="8"/>
         <v>40052</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>99.546875</v>
       </c>
       <c r="G22" s="1">
         <v>185</v>
       </c>
       <c r="H22">
+        <f t="shared" si="8"/>
+        <v>47360</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="9"/>
-        <v>47360</v>
-      </c>
-      <c r="I22">
+        <v>18176</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="10"/>
-        <v>18176</v>
-      </c>
-      <c r="J22">
+        <v>11059200</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="11"/>
-        <v>11059200</v>
-      </c>
-      <c r="K22">
+        <v>1.6435185185185185E-3</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="12"/>
-        <v>1.6435185185185185E-3</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="13"/>
         <v>304.22535211267603</v>
       </c>
     </row>
@@ -842,38 +916,38 @@
         <v>10000</v>
       </c>
       <c r="D23">
+        <f t="shared" si="6"/>
+        <v>33226</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="7"/>
-        <v>33226</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="8"/>
         <v>32310</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>129.7890625</v>
       </c>
       <c r="G23" s="1">
         <v>213</v>
       </c>
       <c r="H23">
+        <f t="shared" si="8"/>
+        <v>54528</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="9"/>
-        <v>54528</v>
-      </c>
-      <c r="I23">
+        <v>11008</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="10"/>
-        <v>11008</v>
-      </c>
-      <c r="J23">
+        <v>11059200</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="11"/>
-        <v>11059200</v>
-      </c>
-      <c r="K23">
+        <v>9.9537037037037042E-4</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="12"/>
-        <v>9.9537037037037042E-4</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="13"/>
         <v>502.32558139534882</v>
       </c>
     </row>
@@ -888,38 +962,38 @@
         <v>10000</v>
       </c>
       <c r="D24">
+        <f t="shared" si="6"/>
+        <v>40968</v>
+      </c>
+      <c r="E24">
         <f t="shared" si="7"/>
-        <v>40968</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="8"/>
         <v>24568</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>160.03125</v>
       </c>
       <c r="G24" s="1">
         <v>235</v>
       </c>
       <c r="H24">
+        <f t="shared" si="8"/>
+        <v>60160</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="9"/>
-        <v>60160</v>
-      </c>
-      <c r="I24">
+        <v>5376</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="10"/>
-        <v>5376</v>
-      </c>
-      <c r="J24">
+        <v>11059200</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="11"/>
-        <v>11059200</v>
-      </c>
-      <c r="K24">
+        <v>4.861111111111111E-4</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="12"/>
-        <v>4.861111111111111E-4</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="13"/>
         <v>1028.5714285714287</v>
       </c>
     </row>
@@ -934,38 +1008,38 @@
         <v>10000</v>
       </c>
       <c r="D25">
+        <f t="shared" si="6"/>
+        <v>48710</v>
+      </c>
+      <c r="E25">
         <f t="shared" si="7"/>
-        <v>48710</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="8"/>
         <v>16826</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>190.2734375</v>
       </c>
       <c r="G25" s="1">
         <v>245</v>
       </c>
       <c r="H25">
+        <f t="shared" si="8"/>
+        <v>62720</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="9"/>
-        <v>62720</v>
-      </c>
-      <c r="I25">
+        <v>2816</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="10"/>
-        <v>2816</v>
-      </c>
-      <c r="J25">
+        <v>11059200</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="11"/>
-        <v>11059200</v>
-      </c>
-      <c r="K25">
+        <v>2.5462962962962961E-4</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="12"/>
-        <v>2.5462962962962961E-4</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="13"/>
         <v>1963.6363636363637</v>
       </c>
     </row>
@@ -980,38 +1054,38 @@
         <v>10000</v>
       </c>
       <c r="D26">
+        <f t="shared" si="6"/>
+        <v>56452</v>
+      </c>
+      <c r="E26">
         <f t="shared" si="7"/>
-        <v>56452</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="8"/>
         <v>9084</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>220.515625</v>
       </c>
       <c r="G26" s="1">
         <v>249</v>
       </c>
       <c r="H26">
+        <f t="shared" si="8"/>
+        <v>63744</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="9"/>
-        <v>63744</v>
-      </c>
-      <c r="I26">
+        <v>1792</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="10"/>
-        <v>1792</v>
-      </c>
-      <c r="J26">
+        <v>11059200</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="11"/>
-        <v>11059200</v>
-      </c>
-      <c r="K26">
+        <v>1.6203703703703703E-4</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="12"/>
-        <v>1.6203703703703703E-4</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="13"/>
         <v>3085.7142857142858</v>
       </c>
     </row>
@@ -1026,7 +1100,7 @@
         <v>10000</v>
       </c>
       <c r="D27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>64194</v>
       </c>
       <c r="E27">
@@ -1034,30 +1108,30 @@
         <v>1342</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>250.7578125</v>
       </c>
       <c r="G27" s="1">
         <v>251</v>
       </c>
       <c r="H27">
+        <f t="shared" si="8"/>
+        <v>64256</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="9"/>
-        <v>64256</v>
-      </c>
-      <c r="I27">
+        <v>1280</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="10"/>
-        <v>1280</v>
-      </c>
-      <c r="J27">
+        <v>11059200</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="11"/>
-        <v>11059200</v>
-      </c>
-      <c r="K27">
+        <v>1.1574074074074075E-4</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="12"/>
-        <v>1.1574074074074075E-4</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="13"/>
         <v>4320</v>
       </c>
     </row>

</xml_diff>